<commit_message>
comienzo gráfica estúpida 1
</commit_message>
<xml_diff>
--- a/shiny/datos/setup/parametros.xlsx
+++ b/shiny/datos/setup/parametros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelishka\Documents\repositorios\cuervo\shiny\datos\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F59783-D729-45C8-B59E-3E92D9EF05A8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE457425-0F66-403B-874B-FF25779919DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="1080" windowWidth="28770" windowHeight="8565" xr2:uid="{727C43C5-BCE5-4B0D-93A1-D5851317154D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>domestico_fechas</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Fe.Creación</t>
   </si>
   <si>
-    <t>Fe.Pre.Entr.</t>
-  </si>
-  <si>
     <t>Fecha Are</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>Fecha factura</t>
-  </si>
-  <si>
-    <t>Fe.Orig.Pref</t>
   </si>
   <si>
     <t>domestico_filtros</t>
@@ -554,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F281DBE1-B0B0-447D-85C8-D5FA6B29FE3C}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,40 +565,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
       <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
-        <v>21</v>
-      </c>
       <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
         <v>32</v>
-      </c>
-      <c r="N1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -615,16 +609,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -636,81 +630,78 @@
         <v>4</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="O3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="1"/>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -720,9 +711,6 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -734,12 +722,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ya hay 3 gráficas
</commit_message>
<xml_diff>
--- a/shiny/datos/setup/parametros.xlsx
+++ b/shiny/datos/setup/parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelishka\Documents\repositorios\cuervo\shiny\datos\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC500ACD-B64B-4D50-9858-0694170CD6E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5683D47-0B1A-4023-B485-A0F9B9201E5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1080" windowWidth="28770" windowHeight="8565" xr2:uid="{727C43C5-BCE5-4B0D-93A1-D5851317154D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{727C43C5-BCE5-4B0D-93A1-D5851317154D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>domestico_fechas</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Fecha Planeación Transporte</t>
   </si>
   <si>
-    <t>Fecha Entrega</t>
-  </si>
-  <si>
     <t>Fec. Entrega a Cte.</t>
   </si>
   <si>
@@ -145,6 +142,30 @@
   </si>
   <si>
     <t>Zona de ventas</t>
+  </si>
+  <si>
+    <t>Ctd.Factura 9Lit</t>
+  </si>
+  <si>
+    <t>Acuse</t>
+  </si>
+  <si>
+    <t>Fe.Orig.Pref</t>
+  </si>
+  <si>
+    <t>Fe.Pre.Entr.</t>
+  </si>
+  <si>
+    <t>Fecha Disponibilidad</t>
+  </si>
+  <si>
+    <t>domestico_fechas_benchmark</t>
+  </si>
+  <si>
+    <t>usa_fechas_benchmark</t>
+  </si>
+  <si>
+    <t>row_fechas_benchmark</t>
   </si>
 </sst>
 </file>
@@ -212,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -228,6 +249,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -543,15 +567,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F281DBE1-B0B0-447D-85C8-D5FA6B29FE3C}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -562,43 +590,52 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
       <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -608,120 +645,147 @@
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="O2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="J3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="J4" s="1"/>
-      <c r="N4" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="M4" s="1"/>
+      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>13</v>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J10" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="5"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>